<commit_message>
#1440 change surveySeries to studySeries
</commit_message>
<xml_diff>
--- a/data/study/study.xlsx
+++ b/data/study/study.xlsx
@@ -36,12 +36,6 @@
     <t>institution.en</t>
   </si>
   <si>
-    <t>surveySeries.de</t>
-  </si>
-  <si>
-    <t>surveySeries.en</t>
-  </si>
-  <si>
     <t>sponsor.de</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   <si>
     <t xml:space="preserve">Das DZHW-Absolventenpanel 2009 ist Teil der DZHW-Absolventenstudienreihe, in der anhand von standardisierten Befragungen Informationen zu Studium, Berufseintritt, Berufsverlauf und Weiterqualifizierung von Hochschulabsolvent(inn)en erfasst werden. Das erste Absolventenpanel wurde 1989 durchgeführt, seitdem wird jeder vierte Absolvent(inn)enjahrgang (Kohorte) untersucht. Für jede Absolvent(inn)enkohorte werden mehrere Befragungswellen durchgeführt, wobei jede Welle in unterschiedlichem zeitlichen Abstand zum Studienabschluss stattfindet. Beim Absolventenpanel 2009 handelt es sich um die sechste Absolvent(inn)enkohorte der Studienreihe. Wie bei der Absolvent(inn)enkohorte 2005 ist die Studienphase der Kohorte 2009 durch den Hochschulwandel im Rahmen des Bologna-Prozesses geprägt und die berufliche Einstiegsphase durch die Wirtschafts- und Finanzkrise im Jahr 2008 gekennzeichnet. Im Unterschied zu vorangegangenen Absolvent(inn)enkohorten weist die Absolvent(inn)enkohorte 2009 jedoch neben Absolvent(inn)en mit traditionellen Abschlüssen auch eine große Anzahl an Bachelorabsolvent(inn)en auf. Eine methodische Neuerung der Absolvent(inn)enkohorte 2009 ist im Vergleich zu den vorangegangen Kohorten außerdem, dass die zweite Befragungswelle erstmals online durchgeführt wurde. Zudem umfasst die zweite Befragungswelle neben einer Hauptbefragung auch zwei Vertiefungsbefragungen zu den Themen „Promotion“ und „regionale Mobilität“.
 </t>
+  </si>
+  <si>
+    <t>studySeries.en</t>
+  </si>
+  <si>
+    <t>studySeries.de</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,78 +717,78 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -817,62 +817,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -903,16 +903,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -921,53 +921,53 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>